<commit_message>
Added version with neural network and his result
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofia/github/movieRecommendation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f0da054e76bb5fa/Desktop/movieRecommendation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053E176E-1B63-8D46-A957-7F5384538C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{053E176E-1B63-8D46-A957-7F5384538C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB22371C-54E6-4813-B55A-762B366A34F6}"/>
   <bookViews>
-    <workbookView xWindow="25660" yWindow="2140" windowWidth="33440" windowHeight="17780" xr2:uid="{4D56E1D2-73D2-443A-B7D4-05BE3F57FE16}"/>
+    <workbookView xWindow="336" yWindow="1392" windowWidth="22140" windowHeight="7224" xr2:uid="{4D56E1D2-73D2-443A-B7D4-05BE3F57FE16}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Specific of the algorithm</t>
   </si>
@@ -174,20 +174,56 @@
     <t xml:space="preserve">Same above + timestamp </t>
   </si>
   <si>
-    <t>0.927</t>
-  </si>
-  <si>
     <t>0.873</t>
   </si>
   <si>
-    <t>0.880</t>
+    <t>0.918</t>
+  </si>
+  <si>
+    <t>0.889</t>
+  </si>
+  <si>
+    <t>0.881</t>
+  </si>
+  <si>
+    <t>20min riordino + 2.10h</t>
+  </si>
+  <si>
+    <t>0.879</t>
+  </si>
+  <si>
+    <t>NN, ReLu and Xen</t>
+  </si>
+  <si>
+    <t>0.196</t>
+  </si>
+  <si>
+    <t>0.842</t>
+  </si>
+  <si>
+    <t>0.658</t>
+  </si>
+  <si>
+    <t>0.739</t>
+  </si>
+  <si>
+    <t>0.260</t>
+  </si>
+  <si>
+    <t>0.902</t>
+  </si>
+  <si>
+    <t>0.477</t>
+  </si>
+  <si>
+    <t>0.624</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +243,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFD5D5D5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -274,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,7 +338,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -624,29 +661,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBE30B6-174B-4D04-B680-50EB1F7A4B2A}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="70.1640625" customWidth="1"/>
+    <col min="1" max="1" width="70.109375" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1"/>
-    <col min="7" max="7" width="28.5" customWidth="1"/>
-    <col min="8" max="8" width="44.5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="13" max="14" width="11.1640625" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="11.5" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="44.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="13" max="14" width="11.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="18" max="18" width="12.77734375" customWidth="1"/>
+    <col min="19" max="19" width="11.44140625" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -881,13 +918,13 @@
       <c r="E7" s="3">
         <v>200</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="14">
         <v>3549907</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="14">
         <v>2186491</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="14">
         <v>5820669</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -976,13 +1013,13 @@
       <c r="E9" s="3">
         <v>200</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="14">
         <v>3549907</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="14">
         <v>2186491</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="14">
         <v>5820669</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -1023,7 +1060,7 @@
       </c>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="19">
+    <row r="10" spans="1:21">
       <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
@@ -1040,30 +1077,104 @@
       <c r="E10" s="13">
         <v>200</v>
       </c>
+      <c r="F10" s="14">
+        <v>2576593</v>
+      </c>
+      <c r="G10" s="14">
+        <v>3198219</v>
+      </c>
       <c r="H10" s="14">
-        <v>5283463</v>
-      </c>
-      <c r="N10">
+        <v>5598976</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="2">
         <v>100</v>
       </c>
-      <c r="O10" t="str">
+      <c r="O10" s="2" t="str">
         <f>O9</f>
         <v>Adaptive(0.01 , 200)</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q10" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" t="s">
-        <v>47</v>
-      </c>
-      <c r="S10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T10" t="s">
-        <v>48</v>
+      <c r="S10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="15">
+        <v>161</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1664830</v>
+      </c>
+      <c r="I12" s="16">
+        <v>1741</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="15">
+        <v>100</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="16">
+        <v>1329</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="T12" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated latex and results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f0da054e76bb5fa/Desktop/movieRecommendation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{053E176E-1B63-8D46-A957-7F5384538C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB22371C-54E6-4813-B55A-762B366A34F6}"/>
+  <xr:revisionPtr revIDLastSave="726" documentId="13_ncr:1_{053E176E-1B63-8D46-A957-7F5384538C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BB41C13-DA06-4DDB-8630-0A79C4BF6632}"/>
   <bookViews>
     <workbookView xWindow="336" yWindow="1392" windowWidth="22140" windowHeight="7224" xr2:uid="{4D56E1D2-73D2-443A-B7D4-05BE3F57FE16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="175">
   <si>
     <t>Specific of the algorithm</t>
   </si>
@@ -192,31 +192,373 @@
     <t>0.879</t>
   </si>
   <si>
-    <t>NN, ReLu and Xen</t>
-  </si>
-  <si>
-    <t>0.196</t>
-  </si>
-  <si>
     <t>0.842</t>
   </si>
   <si>
-    <t>0.658</t>
-  </si>
-  <si>
-    <t>0.739</t>
-  </si>
-  <si>
-    <t>0.260</t>
-  </si>
-  <si>
-    <t>0.902</t>
-  </si>
-  <si>
-    <t>0.477</t>
-  </si>
-  <si>
-    <t>0.624</t>
+    <t>0.894</t>
+  </si>
+  <si>
+    <t>0.837</t>
+  </si>
+  <si>
+    <t>0.718</t>
+  </si>
+  <si>
+    <t>0.827</t>
+  </si>
+  <si>
+    <t>0.833</t>
+  </si>
+  <si>
+    <t>0.079</t>
+  </si>
+  <si>
+    <t>0.834</t>
+  </si>
+  <si>
+    <t>0.778</t>
+  </si>
+  <si>
+    <t>0.831</t>
+  </si>
+  <si>
+    <t>0.727</t>
+  </si>
+  <si>
+    <t>0.847</t>
+  </si>
+  <si>
+    <t>0.854</t>
+  </si>
+  <si>
+    <t>0.726</t>
+  </si>
+  <si>
+    <t>0.850</t>
+  </si>
+  <si>
+    <t>0.784</t>
+  </si>
+  <si>
+    <t>0.096</t>
+  </si>
+  <si>
+    <t>0.843</t>
+  </si>
+  <si>
+    <t>0.682</t>
+  </si>
+  <si>
+    <t>0.754</t>
+  </si>
+  <si>
+    <t>0.139</t>
+  </si>
+  <si>
+    <t>0.576</t>
+  </si>
+  <si>
+    <t>Collaborative(avg common, at least 2) + content filtering (avg between them)</t>
+  </si>
+  <si>
+    <t>0.484</t>
+  </si>
+  <si>
+    <t>0.029</t>
+  </si>
+  <si>
+    <t>0.832</t>
+  </si>
+  <si>
+    <t>0.742</t>
+  </si>
+  <si>
+    <t>0.785</t>
+  </si>
+  <si>
+    <t>0.089</t>
+  </si>
+  <si>
+    <t>0.731</t>
+  </si>
+  <si>
+    <t>0.054</t>
+  </si>
+  <si>
+    <t>0.771</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>0.531</t>
+  </si>
+  <si>
+    <t>0.653</t>
+  </si>
+  <si>
+    <t>0.133</t>
+  </si>
+  <si>
+    <t>0.865</t>
+  </si>
+  <si>
+    <t>0.501</t>
+  </si>
+  <si>
+    <t>0.208</t>
+  </si>
+  <si>
+    <t>0.861</t>
+  </si>
+  <si>
+    <t>0.803</t>
+  </si>
+  <si>
+    <t>0.986</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>0.868</t>
+  </si>
+  <si>
+    <t>0.929</t>
+  </si>
+  <si>
+    <t>0.899</t>
+  </si>
+  <si>
+    <t>0.962</t>
+  </si>
+  <si>
+    <t>0.431</t>
+  </si>
+  <si>
+    <t>0.870</t>
+  </si>
+  <si>
+    <t>0.849</t>
+  </si>
+  <si>
+    <t>0.859</t>
+  </si>
+  <si>
+    <t>No value inserted</t>
+  </si>
+  <si>
+    <t>NN, Swish and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95 , SGD</t>
+  </si>
+  <si>
+    <t>0.424</t>
+  </si>
+  <si>
+    <t>0.768</t>
+  </si>
+  <si>
+    <t>0.972</t>
+  </si>
+  <si>
+    <t>0.860</t>
+  </si>
+  <si>
+    <t>0.946</t>
+  </si>
+  <si>
+    <t>0.394</t>
+  </si>
+  <si>
+    <t>0.874</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>0.279</t>
+  </si>
+  <si>
+    <t>0.817</t>
+  </si>
+  <si>
+    <t>0.428</t>
+  </si>
+  <si>
+    <t>0.920</t>
+  </si>
+  <si>
+    <t>0.670</t>
+  </si>
+  <si>
+    <t>0.775</t>
+  </si>
+  <si>
+    <t>NN, tanh and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95 , SGD</t>
+  </si>
+  <si>
+    <t>0.965</t>
+  </si>
+  <si>
+    <t>0.872</t>
+  </si>
+  <si>
+    <t>0.998</t>
+  </si>
+  <si>
+    <t>0.930</t>
+  </si>
+  <si>
+    <t>0.138</t>
+  </si>
+  <si>
+    <t>0.876</t>
+  </si>
+  <si>
+    <t>0.981</t>
+  </si>
+  <si>
+    <t>0.415</t>
+  </si>
+  <si>
+    <t>0.714</t>
+  </si>
+  <si>
+    <t>0.798</t>
+  </si>
+  <si>
+    <t>NN, ReLu and Xen (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95 , SGD</t>
+  </si>
+  <si>
+    <t>NN, ReLu and Xen (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>NN, Swish and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95 , Momentum</t>
+  </si>
+  <si>
+    <t>NN, Swish and MSE (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95 , Momentum</t>
+  </si>
+  <si>
+    <t>NN, ReLu and Xen (20 , 32 , 16 , 16 ,  10), diff threshold 0.3 , 0.95 , Momentum</t>
+  </si>
+  <si>
+    <t>NN, ReLu and Xen (20 , 32 , 16 , 16 ,  10), threshold 0.5 , 0.95 , Momentum</t>
+  </si>
+  <si>
+    <t>NN, tanh and Xen (20 , 32 , 16,  10), threshold 0.4 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>NN, tanh and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>NN, tanh and MSE (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>0.996</t>
+  </si>
+  <si>
+    <t>0.374</t>
+  </si>
+  <si>
+    <t>0.863</t>
+  </si>
+  <si>
+    <t>NN, tanh and MSE (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.95, SGD</t>
+  </si>
+  <si>
+    <t>0.992</t>
+  </si>
+  <si>
+    <t>0.313</t>
+  </si>
+  <si>
+    <t>0.858</t>
+  </si>
+  <si>
+    <t>0.922</t>
+  </si>
+  <si>
+    <t>0.438</t>
+  </si>
+  <si>
+    <t>0.907</t>
+  </si>
+  <si>
+    <t>0.710</t>
+  </si>
+  <si>
+    <t>0.796</t>
+  </si>
+  <si>
+    <t>0.117</t>
+  </si>
+  <si>
+    <t>0.669</t>
+  </si>
+  <si>
+    <t>NN, Leaky-ReLu and Xen (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95 , SGD</t>
+  </si>
+  <si>
+    <t>NN, Leaky-ReLu and Xen (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>0.183</t>
+  </si>
+  <si>
+    <t>0.749</t>
+  </si>
+  <si>
+    <t>NN, ReLu and MSE (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95, Momentum</t>
+  </si>
+  <si>
+    <t>0.267</t>
+  </si>
+  <si>
+    <t>0.953</t>
+  </si>
+  <si>
+    <t>0.804</t>
+  </si>
+  <si>
+    <t>NN, tanh and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.90 , SGD</t>
+  </si>
+  <si>
+    <t>NN, Swish and Xen (20 , 32 , 16  ,  10), diff threshold 0.3 , 0.90 , Momentum</t>
+  </si>
+  <si>
+    <t>Final results Collaborative + Content-based filtering</t>
+  </si>
+  <si>
+    <t>NN results: first version</t>
+  </si>
+  <si>
+    <t>NN results: second version</t>
+  </si>
+  <si>
+    <t>0.103</t>
+  </si>
+  <si>
+    <t>0.769</t>
+  </si>
+  <si>
+    <t>0.217</t>
+  </si>
+  <si>
+    <t>0.914</t>
+  </si>
+  <si>
+    <t>0.685</t>
+  </si>
+  <si>
+    <t>0.783</t>
+  </si>
+  <si>
+    <t>0.168</t>
+  </si>
+  <si>
+    <t>0.666</t>
+  </si>
+  <si>
+    <t>NN, Leaky-ReLu and MSE (20 , 32 , 16 ,  10), diff threshold 0.3 , 0.95, SGD</t>
   </si>
 </sst>
 </file>
@@ -245,7 +587,7 @@
       <name val="Var(--jp-code-font-family)"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +603,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +699,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -661,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBE30B6-174B-4D04-B680-50EB1F7A4B2A}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1127,54 +1496,1224 @@
         <v>50</v>
       </c>
     </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
     <row r="12" spans="1:21">
-      <c r="A12" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="18"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>161</v>
+      </c>
+      <c r="E15" s="3">
+        <v>200</v>
+      </c>
+      <c r="F15" s="8">
+        <v>3549907</v>
+      </c>
+      <c r="G15" s="8">
+        <v>2186491</v>
+      </c>
+      <c r="H15" s="8">
+        <v>5820669</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="3">
+        <v>100</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5">
+        <v>161</v>
+      </c>
+      <c r="E16" s="5">
+        <v>200</v>
+      </c>
+      <c r="F16" s="6">
+        <v>3549907</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2186491</v>
+      </c>
+      <c r="H16" s="6">
+        <v>5820669</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="5">
+        <v>100</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <v>200</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8">
+        <v>4892329</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N17" s="3">
+        <v>100</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="3">
+        <v>161</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8">
+        <v>3549907</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="3">
+        <v>100</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" s="9">
+        <v>1347</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="B19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="10">
+        <v>161</v>
+      </c>
+      <c r="E23" s="7">
+        <v>200</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="3">
+        <v>5021303</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1526</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N23" s="3">
+        <v>100</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P23" s="9">
+        <v>1439</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="10">
+        <v>161</v>
+      </c>
+      <c r="E24" s="7">
+        <v>200</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="3">
+        <v>4815341</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1486</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N24" s="3">
+        <v>100</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="9">
+        <v>1411</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5">
+        <v>161</v>
+      </c>
+      <c r="E25" s="4">
+        <v>200</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5">
+        <v>3006413</v>
+      </c>
+      <c r="I25" s="21">
+        <v>1037</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N25" s="5">
+        <v>300</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P25" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10">
+        <v>161</v>
+      </c>
+      <c r="E26" s="7">
+        <v>200</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="3">
+        <v>209611</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N26" s="3">
+        <v>500</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" s="9">
+        <v>1263</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="T26" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="10">
+        <v>161</v>
+      </c>
+      <c r="E27" s="7">
+        <v>200</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="3">
+        <v>210311</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N27" s="3">
+        <v>500</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P27" s="9">
+        <v>1263</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="10">
+        <v>161</v>
+      </c>
+      <c r="E29" s="7">
+        <v>200</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="3">
+        <v>2823090</v>
+      </c>
+      <c r="I29" s="9">
+        <v>1829</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10">
+        <v>161</v>
+      </c>
+      <c r="E30" s="7">
+        <v>200</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="3">
+        <v>3059942</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1790</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" s="3">
+        <v>100</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" s="9">
+        <v>1585</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="S30" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="T30" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="10">
+        <v>161</v>
+      </c>
+      <c r="E32" s="7">
+        <v>200</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="3">
+        <v>522540</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="N32" s="3">
+        <v>500</v>
+      </c>
+      <c r="O32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" s="9">
+        <v>1074</v>
+      </c>
+      <c r="Q32" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="R32" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="S32" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T32" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="10">
+        <v>161</v>
+      </c>
+      <c r="E33" s="7">
+        <v>200</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="3">
+        <v>2470977</v>
+      </c>
+      <c r="I33" s="9">
+        <v>1563</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="15">
-        <v>161</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1664830</v>
-      </c>
-      <c r="I12" s="16">
-        <v>1741</v>
-      </c>
-      <c r="J12" s="15" t="s">
+      <c r="N33" s="3">
+        <v>100</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" s="9">
+        <v>1297</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="T33" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="10">
+        <v>161</v>
+      </c>
+      <c r="E34" s="7">
+        <v>200</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="5">
+        <v>161</v>
+      </c>
+      <c r="E36" s="4">
+        <v>200</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5">
+        <v>2972631</v>
+      </c>
+      <c r="I36" s="21">
+        <v>1240</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N36" s="5">
+        <v>100</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P36" s="21">
+        <v>1138</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="10">
+        <v>161</v>
+      </c>
+      <c r="E37" s="7">
+        <v>200</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="10">
+        <v>161</v>
+      </c>
+      <c r="E38" s="7">
+        <v>200</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="3">
+        <v>653846</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N38" s="3">
+        <v>500</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P38" s="9">
+        <v>1135</v>
+      </c>
+      <c r="Q38" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="R38" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S38" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="T38" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="H39" s="2"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="15">
+        <v>161</v>
+      </c>
+      <c r="E40">
+        <v>200</v>
+      </c>
+      <c r="H40" s="2">
+        <v>590897</v>
+      </c>
+      <c r="I40" s="16">
+        <v>1156</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="15" t="s">
+      <c r="N40" s="2">
+        <v>500</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" s="16">
+        <v>1043</v>
+      </c>
+      <c r="Q40" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="R40" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S40" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="T40" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="15">
+        <v>161</v>
+      </c>
+      <c r="E41">
+        <v>200</v>
+      </c>
+      <c r="H41" s="15">
+        <v>2905429</v>
+      </c>
+      <c r="I41" s="16">
+        <v>1629</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L41" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="15">
-        <v>100</v>
-      </c>
-      <c r="O12" s="15" t="s">
+      <c r="M41" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="N41" s="15">
+        <v>250</v>
+      </c>
+      <c r="O41" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="16">
-        <v>1329</v>
-      </c>
-      <c r="Q12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S12" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T12" s="15" t="s">
-        <v>60</v>
+      <c r="P41" s="16">
+        <v>1372</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="15">
+        <v>161</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="5">
+        <v>161</v>
+      </c>
+      <c r="E47" s="4">
+        <v>200</v>
+      </c>
+      <c r="H47" s="2">
+        <v>715564</v>
+      </c>
+      <c r="I47" s="16">
+        <v>1199</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="5">
+        <v>161</v>
+      </c>
+      <c r="E49" s="4">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>